<commit_message>
Add a case when serviceInterface has annotations but serviceImpl doesn't have
</commit_message>
<xml_diff>
--- a/Results as a table.xlsx
+++ b/Results as a table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\spring-boot-validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D563B90-9962-4FEC-B87C-A036F6AF517B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383931B1-D7FA-404A-A693-4DB6B1FDED4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{8C6F6555-6C19-4AD6-9297-B9390D6A4920}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Где валидация</t>
   </si>
@@ -96,7 +96,10 @@
     <t>В контроллере можно не ставить над классом @Validated, если не надо валидировать переменные пути и параметров метода</t>
   </si>
   <si>
-    <t>Если сервис объявлен как интерфейс, то надо иметь валидационные аннотации и в интерфейсе и в классе имплементации</t>
+    <t>Сервис как интерфейс с аннотациями валидации + Impl c @Validated, но без аннотаций на параметрах метода</t>
+  </si>
+  <si>
+    <t>Если сервис объявлен как интерфейс, то надо иметь валидационные аннотации в интерфейсе (в классе имплементации не обязательно)</t>
   </si>
 </sst>
 </file>
@@ -139,15 +142,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -168,16 +177,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -192,8 +191,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEA02EE8-CF31-449D-A43F-D6A51E81DBB8}" name="Таблица1" displayName="Таблица1" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7" xr:uid="{BEA02EE8-CF31-449D-A43F-D6A51E81DBB8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BEA02EE8-CF31-449D-A43F-D6A51E81DBB8}" name="Таблица1" displayName="Таблица1" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{BEA02EE8-CF31-449D-A43F-D6A51E81DBB8}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0157DBD7-2685-4463-A177-416E67EE1DB5}" name="Где валидация"/>
     <tableColumn id="2" xr3:uid="{8D60A4B8-7B1B-47F0-8DC7-6B5909AC661C}" name="Кейс"/>
@@ -502,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D552D835-7914-469E-A6DC-49A04B22FF85}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -636,22 +635,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +708,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C2:E7</xm:sqref>
+          <xm:sqref>C2:E8</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>